<commit_message>
moving on to abstract
</commit_message>
<xml_diff>
--- a/report/Tables/GLPF site characteristics.xlsx
+++ b/report/Tables/GLPF site characteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\GLPF_manuscript\report\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE7DF6DF-9C10-4BAF-AC22-3190D2BE6507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1DEA21-8609-45D3-8A1A-0C5CED309662}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="480" windowWidth="22995" windowHeight="14910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="555" windowWidth="22995" windowHeight="14910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Sites" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -521,21 +523,6 @@
     <t>15 (16)</t>
   </si>
   <si>
-    <t>UW</t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>CG</t>
-  </si>
-  <si>
-    <t>BK</t>
-  </si>
-  <si>
     <t>Menominee</t>
   </si>
   <si>
@@ -651,6 +638,21 @@
   </si>
   <si>
     <t>Ontario</t>
+  </si>
+  <si>
+    <t>Underwood</t>
+  </si>
+  <si>
+    <t>Wauwatosa</t>
+  </si>
+  <si>
+    <t>16th</t>
+  </si>
+  <si>
+    <t>Cedarburg</t>
+  </si>
+  <si>
+    <t>Bark</t>
   </si>
 </sst>
 </file>
@@ -662,7 +664,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,6 +739,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -841,7 +849,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1023,6 +1031,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1388,32 +1397,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -1422,535 +1427,577 @@
         <v>21</v>
       </c>
       <c r="E1" s="49" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G1" s="50" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="71" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="67" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C2" s="54" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F2" s="51">
         <v>3.8</v>
       </c>
-      <c r="G2" s="68">
+      <c r="G2" s="69">
         <v>3.1</v>
       </c>
-      <c r="H2" s="68">
+      <c r="H2" s="69">
         <v>52.2</v>
       </c>
-      <c r="I2" s="68">
+      <c r="I2" s="69">
         <v>20.6</v>
       </c>
-      <c r="J2" s="68">
+      <c r="J2" s="69">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C3" s="55" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F3" s="51">
         <v>6.3</v>
       </c>
-      <c r="G3" s="68">
+      <c r="G3" s="69">
         <v>69.599999999999994</v>
       </c>
-      <c r="H3" s="68">
+      <c r="H3" s="69">
         <v>4.2</v>
       </c>
-      <c r="I3" s="68">
+      <c r="I3" s="69">
         <v>7.4</v>
       </c>
-      <c r="J3" s="68">
+      <c r="J3" s="69">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="51"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C4" s="55" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F4" s="51">
         <v>29.4</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="69">
         <v>41.5</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="69">
         <v>11</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="69">
         <v>4.2</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="69">
         <v>11.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="51"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C5" s="55" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F5" s="51">
         <v>51.5</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="69">
         <v>18.899999999999999</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="69">
         <v>14.9</v>
       </c>
-      <c r="I5" s="68">
+      <c r="I5" s="69">
         <v>6.5</v>
       </c>
-      <c r="J5" s="68">
+      <c r="J5" s="69">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="51"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C6" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F6" s="51">
         <v>92</v>
       </c>
-      <c r="G6" s="68">
+      <c r="G6" s="69">
         <v>0.2</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="69">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I6" s="68">
+      <c r="I6" s="69">
         <v>1.9</v>
       </c>
-      <c r="J6" s="68">
+      <c r="J6" s="69">
         <v>33.799999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="51"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B7" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C7" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F7" s="51">
         <v>10.4</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="69">
         <v>66.900000000000006</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="69">
         <v>10.8</v>
       </c>
-      <c r="I7" s="68">
+      <c r="I7" s="69">
         <v>3.5</v>
       </c>
-      <c r="J7" s="68">
+      <c r="J7" s="69">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="51"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C8" s="55" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F8" s="51">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="69">
         <v>78.900000000000006</v>
       </c>
-      <c r="H8" s="68">
+      <c r="H8" s="69">
         <v>6.5</v>
       </c>
-      <c r="I8" s="68">
+      <c r="I8" s="69">
         <v>1.3</v>
       </c>
-      <c r="J8" s="68">
+      <c r="J8" s="69">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="51"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B9" s="53" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C9" s="55" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="53" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F9" s="51">
         <v>9</v>
       </c>
-      <c r="G9" s="68">
+      <c r="G9" s="69">
         <v>84.5</v>
       </c>
-      <c r="H9" s="68">
+      <c r="H9" s="69">
         <v>4.7</v>
       </c>
-      <c r="I9" s="68">
+      <c r="I9" s="69">
         <v>0.5</v>
       </c>
-      <c r="J9" s="68">
+      <c r="J9" s="69">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="51"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C10" s="59" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="F10" s="51">
         <v>88.9</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="69">
         <v>1.2</v>
       </c>
-      <c r="H10" s="68">
+      <c r="H10" s="69">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I10" s="68">
+      <c r="I10" s="69">
         <v>2</v>
       </c>
-      <c r="J10" s="68">
+      <c r="J10" s="69">
         <v>29.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="51"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C11" s="60" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="F11" s="51">
         <v>65</v>
       </c>
-      <c r="G11" s="68">
+      <c r="G11" s="69">
         <v>18.100000000000001</v>
       </c>
-      <c r="H11" s="68">
+      <c r="H11" s="69">
         <v>5.6</v>
       </c>
-      <c r="I11" s="68">
+      <c r="I11" s="69">
         <v>1.9</v>
       </c>
-      <c r="J11" s="68">
+      <c r="J11" s="69">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="51"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C12" s="60" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="F12" s="51">
         <v>67.7</v>
       </c>
-      <c r="G12" s="68">
+      <c r="G12" s="69">
         <v>16.600000000000001</v>
       </c>
-      <c r="H12" s="68">
+      <c r="H12" s="69">
         <v>5.2</v>
       </c>
-      <c r="I12" s="68">
+      <c r="I12" s="69">
         <v>1.7</v>
       </c>
-      <c r="J12" s="68">
+      <c r="J12" s="69">
         <v>28.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="51"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C13" s="55" t="s">
         <v>57</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="F13" s="51">
         <v>11.6</v>
       </c>
-      <c r="G13" s="68">
+      <c r="G13" s="69">
         <v>53.5</v>
       </c>
-      <c r="H13" s="68">
+      <c r="H13" s="69">
         <v>13.3</v>
       </c>
-      <c r="I13" s="68">
+      <c r="I13" s="69">
         <v>5.2</v>
       </c>
-      <c r="J13" s="68">
+      <c r="J13" s="69">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="51"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C14" s="55" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="F14" s="51">
         <v>32.200000000000003</v>
       </c>
-      <c r="G14" s="68">
+      <c r="G14" s="69">
         <v>35.200000000000003</v>
       </c>
-      <c r="H14" s="68">
+      <c r="H14" s="69">
         <v>15.5</v>
       </c>
-      <c r="I14" s="68">
+      <c r="I14" s="69">
         <v>4.2</v>
       </c>
-      <c r="J14" s="68">
+      <c r="J14" s="69">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="51"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C15" s="55" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="53" t="s">
         <v>107</v>
-      </c>
-      <c r="E15" s="53" t="s">
-        <v>112</v>
       </c>
       <c r="F15" s="51">
         <v>98.4</v>
       </c>
-      <c r="G15" s="68">
+      <c r="G15" s="69">
         <v>0.3</v>
       </c>
-      <c r="H15" s="68">
+      <c r="H15" s="69">
         <v>0.6</v>
       </c>
-      <c r="I15" s="68">
+      <c r="I15" s="69">
         <v>0.1</v>
       </c>
-      <c r="J15" s="68">
+      <c r="J15" s="69">
         <v>51.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="51"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="57" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C16" s="55" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F16" s="61">
         <v>52.5</v>
       </c>
-      <c r="G16" s="69">
+      <c r="G16" s="70">
         <v>24.1</v>
       </c>
-      <c r="H16" s="69">
+      <c r="H16" s="70">
         <v>16.600000000000001</v>
       </c>
-      <c r="I16" s="69">
+      <c r="I16" s="70">
         <v>1.6</v>
       </c>
-      <c r="J16" s="68">
+      <c r="J16" s="69">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="51"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C17" s="64" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E17" s="65" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F17" s="66">
         <v>48</v>
       </c>
-      <c r="G17" s="70">
+      <c r="G17" s="71">
         <v>23.9</v>
       </c>
-      <c r="H17" s="70">
+      <c r="H17" s="71">
         <v>13.6</v>
       </c>
-      <c r="I17" s="70">
+      <c r="I17" s="71">
         <v>0.5</v>
       </c>
-      <c r="J17" s="70">
+      <c r="J17" s="71">
         <v>18.3</v>
       </c>
+      <c r="K17" s="51"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1986,23 +2033,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2047,17 +2094,17 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="75" t="s">
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="75"/>
+      <c r="O4" s="76"/>
     </row>
     <row r="5" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">

</xml_diff>

<commit_message>
more peer review revisions
</commit_message>
<xml_diff>
--- a/report/Tables/GLPF site characteristics.xlsx
+++ b/report/Tables/GLPF site characteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\GLPF_manuscript\report\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1DEA21-8609-45D3-8A1A-0C5CED309662}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F979125-43E1-4234-BF1B-620AD6C34BF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="555" windowWidth="22995" windowHeight="14910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="150" windowWidth="28305" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Sites" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="142">
   <si>
     <t>USGS station ID</t>
   </si>
@@ -654,6 +654,31 @@
   <si>
     <t>Bark</t>
   </si>
+  <si>
+    <r>
+      <t>Drainage area (km</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>km^2</t>
+  </si>
 </sst>
 </file>
 
@@ -664,7 +689,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,12 +764,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -849,7 +868,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1031,7 +1050,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1397,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,11 +1427,12 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -1429,23 +1448,26 @@
       <c r="E1" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="H1" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="I1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="J1" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="K1" s="67" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>112</v>
       </c>
@@ -1461,24 +1483,27 @@
       <c r="E2" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="51">
+      <c r="F2" s="53">
+        <v>10200</v>
+      </c>
+      <c r="G2" s="51">
         <v>3.8</v>
       </c>
-      <c r="G2" s="69">
+      <c r="H2" s="68">
         <v>3.1</v>
       </c>
-      <c r="H2" s="69">
-        <v>52.2</v>
-      </c>
-      <c r="I2" s="69">
-        <v>20.6</v>
-      </c>
-      <c r="J2" s="69">
+      <c r="I2" s="68">
+        <v>52.6</v>
+      </c>
+      <c r="J2" s="68">
+        <v>37.4</v>
+      </c>
+      <c r="K2" s="68">
         <v>0.5</v>
       </c>
-      <c r="K2" s="51"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="51"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>113</v>
       </c>
@@ -1494,24 +1519,27 @@
       <c r="E3" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="51">
+      <c r="F3" s="53">
+        <v>1360</v>
+      </c>
+      <c r="G3" s="51">
         <v>6.3</v>
       </c>
-      <c r="G3" s="69">
-        <v>69.599999999999994</v>
-      </c>
-      <c r="H3" s="69">
+      <c r="H3" s="68">
+        <v>69.8</v>
+      </c>
+      <c r="I3" s="68">
         <v>4.2</v>
       </c>
-      <c r="I3" s="69">
-        <v>7.4</v>
-      </c>
-      <c r="J3" s="69">
+      <c r="J3" s="68">
+        <v>19.2</v>
+      </c>
+      <c r="K3" s="68">
         <v>1.5</v>
       </c>
-      <c r="K3" s="51"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="51"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>114</v>
       </c>
@@ -1527,24 +1555,27 @@
       <c r="E4" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="51">
-        <v>29.4</v>
-      </c>
-      <c r="G4" s="69">
+      <c r="F4" s="53">
+        <v>2260</v>
+      </c>
+      <c r="G4" s="51">
+        <v>29.3</v>
+      </c>
+      <c r="H4" s="68">
         <v>41.5</v>
       </c>
-      <c r="H4" s="69">
-        <v>11</v>
-      </c>
-      <c r="I4" s="69">
-        <v>4.2</v>
-      </c>
-      <c r="J4" s="69">
-        <v>11.8</v>
-      </c>
-      <c r="K4" s="51"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4" s="68">
+        <v>11.3</v>
+      </c>
+      <c r="J4" s="68">
+        <v>16.8</v>
+      </c>
+      <c r="K4" s="68">
+        <v>11.7</v>
+      </c>
+      <c r="L4" s="51"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>115</v>
       </c>
@@ -1560,24 +1591,27 @@
       <c r="E5" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="51">
-        <v>51.5</v>
-      </c>
-      <c r="G5" s="69">
+      <c r="F5" s="53">
+        <v>1900</v>
+      </c>
+      <c r="G5" s="51">
+        <v>51.4</v>
+      </c>
+      <c r="H5" s="68">
         <v>18.899999999999999</v>
       </c>
-      <c r="H5" s="69">
-        <v>14.9</v>
-      </c>
-      <c r="I5" s="69">
-        <v>6.5</v>
-      </c>
-      <c r="J5" s="69">
-        <v>20.2</v>
-      </c>
-      <c r="K5" s="51"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I5" s="68">
+        <v>15</v>
+      </c>
+      <c r="J5" s="68">
+        <v>13.4</v>
+      </c>
+      <c r="K5" s="68">
+        <v>20</v>
+      </c>
+      <c r="L5" s="51"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>116</v>
       </c>
@@ -1593,24 +1627,27 @@
       <c r="E6" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="53">
+        <v>484</v>
+      </c>
+      <c r="G6" s="51">
         <v>92</v>
       </c>
-      <c r="G6" s="69">
+      <c r="H6" s="68">
         <v>0.2</v>
       </c>
-      <c r="H6" s="69">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I6" s="69">
-        <v>1.9</v>
-      </c>
-      <c r="J6" s="69">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="K6" s="51"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="J6" s="68">
+        <v>3.3</v>
+      </c>
+      <c r="K6" s="68">
+        <v>33.6</v>
+      </c>
+      <c r="L6" s="51"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>117</v>
       </c>
@@ -1626,24 +1663,27 @@
       <c r="E7" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="51">
-        <v>10.4</v>
-      </c>
-      <c r="G7" s="69">
+      <c r="F7" s="53">
+        <v>2700</v>
+      </c>
+      <c r="G7" s="51">
+        <v>10.3</v>
+      </c>
+      <c r="H7" s="68">
         <v>66.900000000000006</v>
       </c>
-      <c r="H7" s="69">
-        <v>10.8</v>
-      </c>
-      <c r="I7" s="69">
-        <v>3.5</v>
-      </c>
-      <c r="J7" s="69">
+      <c r="I7" s="68">
+        <v>10.9</v>
+      </c>
+      <c r="J7" s="68">
+        <v>11.5</v>
+      </c>
+      <c r="K7" s="68">
         <v>2.5</v>
       </c>
-      <c r="K7" s="51"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="51"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
         <v>124</v>
       </c>
@@ -1659,24 +1699,27 @@
       <c r="E8" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="51">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="G8" s="69">
-        <v>78.900000000000006</v>
-      </c>
-      <c r="H8" s="69">
+      <c r="F8" s="53">
+        <v>16400</v>
+      </c>
+      <c r="G8" s="51">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H8" s="68">
+        <v>79</v>
+      </c>
+      <c r="I8" s="68">
         <v>6.5</v>
       </c>
-      <c r="I8" s="69">
-        <v>1.3</v>
-      </c>
-      <c r="J8" s="69">
-        <v>2.5</v>
-      </c>
-      <c r="K8" s="51"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="68">
+        <v>4.3</v>
+      </c>
+      <c r="K8" s="68">
+        <v>2.4</v>
+      </c>
+      <c r="L8" s="51"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>125</v>
       </c>
@@ -1692,24 +1735,27 @@
       <c r="E9" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="51">
-        <v>9</v>
-      </c>
-      <c r="G9" s="69">
-        <v>84.5</v>
-      </c>
-      <c r="H9" s="69">
+      <c r="F9" s="53">
+        <v>1110</v>
+      </c>
+      <c r="G9" s="51">
+        <v>8.9</v>
+      </c>
+      <c r="H9" s="68">
+        <v>84.6</v>
+      </c>
+      <c r="I9" s="68">
         <v>4.7</v>
       </c>
-      <c r="I9" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="J9" s="69">
+      <c r="J9" s="68">
+        <v>1.3</v>
+      </c>
+      <c r="K9" s="68">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K9" s="51"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="51"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
         <v>118</v>
       </c>
@@ -1725,24 +1771,27 @@
       <c r="E10" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="F10" s="51">
-        <v>88.9</v>
-      </c>
-      <c r="G10" s="69">
+      <c r="F10" s="53">
+        <v>46.9</v>
+      </c>
+      <c r="G10" s="51">
+        <v>89.5</v>
+      </c>
+      <c r="H10" s="68">
         <v>1.2</v>
       </c>
-      <c r="H10" s="69">
+      <c r="I10" s="68">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I10" s="69">
-        <v>2</v>
-      </c>
-      <c r="J10" s="69">
-        <v>29.4</v>
-      </c>
-      <c r="K10" s="51"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="68">
+        <v>6</v>
+      </c>
+      <c r="K10" s="68">
+        <v>30.1</v>
+      </c>
+      <c r="L10" s="51"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="s">
         <v>119</v>
       </c>
@@ -1758,24 +1807,27 @@
       <c r="E11" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="F11" s="51">
-        <v>65</v>
-      </c>
-      <c r="G11" s="69">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="H11" s="69">
-        <v>5.6</v>
-      </c>
-      <c r="I11" s="69">
-        <v>1.9</v>
-      </c>
-      <c r="J11" s="69">
-        <v>25.6</v>
-      </c>
-      <c r="K11" s="51"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="53">
+        <v>319</v>
+      </c>
+      <c r="G11" s="51">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="H11" s="68">
+        <v>18.7</v>
+      </c>
+      <c r="I11" s="68">
+        <v>5.7</v>
+      </c>
+      <c r="J11" s="68">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="K11" s="68">
+        <v>25.1</v>
+      </c>
+      <c r="L11" s="51"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="s">
         <v>120</v>
       </c>
@@ -1791,24 +1843,27 @@
       <c r="E12" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="F12" s="51">
-        <v>67.7</v>
-      </c>
-      <c r="G12" s="69">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="H12" s="69">
-        <v>5.2</v>
-      </c>
-      <c r="I12" s="69">
-        <v>1.7</v>
-      </c>
-      <c r="J12" s="69">
-        <v>28.1</v>
-      </c>
-      <c r="K12" s="51"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="53">
+        <v>378</v>
+      </c>
+      <c r="G12" s="51">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="H12" s="68">
+        <v>17.2</v>
+      </c>
+      <c r="I12" s="68">
+        <v>5.3</v>
+      </c>
+      <c r="J12" s="68">
+        <v>8.9</v>
+      </c>
+      <c r="K12" s="68">
+        <v>27.6</v>
+      </c>
+      <c r="L12" s="51"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>121</v>
       </c>
@@ -1824,24 +1879,27 @@
       <c r="E13" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="F13" s="51">
-        <v>11.6</v>
-      </c>
-      <c r="G13" s="69">
+      <c r="F13" s="53">
+        <v>1570</v>
+      </c>
+      <c r="G13" s="51">
+        <v>11.4</v>
+      </c>
+      <c r="H13" s="68">
         <v>53.5</v>
       </c>
-      <c r="H13" s="69">
-        <v>13.3</v>
-      </c>
-      <c r="I13" s="69">
-        <v>5.2</v>
-      </c>
-      <c r="J13" s="69">
-        <v>3.3</v>
-      </c>
-      <c r="K13" s="51"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="68">
+        <v>13.7</v>
+      </c>
+      <c r="J13" s="68">
+        <v>20.7</v>
+      </c>
+      <c r="K13" s="68">
+        <v>3.2</v>
+      </c>
+      <c r="L13" s="51"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
         <v>122</v>
       </c>
@@ -1857,24 +1915,27 @@
       <c r="E14" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="F14" s="51">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="G14" s="69">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="H14" s="69">
-        <v>15.5</v>
-      </c>
-      <c r="I14" s="69">
-        <v>4.2</v>
-      </c>
-      <c r="J14" s="69">
-        <v>5.5</v>
-      </c>
-      <c r="K14" s="51"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="53">
+        <v>78.2</v>
+      </c>
+      <c r="G14" s="51">
+        <v>29.2</v>
+      </c>
+      <c r="H14" s="68">
+        <v>35.1</v>
+      </c>
+      <c r="I14" s="68">
+        <v>15.8</v>
+      </c>
+      <c r="J14" s="68">
+        <v>16.3</v>
+      </c>
+      <c r="K14" s="68">
+        <v>4.7</v>
+      </c>
+      <c r="L14" s="51"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="s">
         <v>123</v>
       </c>
@@ -1890,24 +1951,27 @@
       <c r="E15" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="51">
-        <v>98.4</v>
-      </c>
-      <c r="G15" s="69">
-        <v>0.3</v>
-      </c>
-      <c r="H15" s="69">
-        <v>0.6</v>
-      </c>
-      <c r="I15" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="J15" s="69">
-        <v>51.7</v>
-      </c>
-      <c r="K15" s="51"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="53">
+        <v>47.9</v>
+      </c>
+      <c r="G15" s="51">
+        <v>97.9</v>
+      </c>
+      <c r="H15" s="68">
+        <v>0.4</v>
+      </c>
+      <c r="I15" s="68">
+        <v>0.7</v>
+      </c>
+      <c r="J15" s="68">
+        <v>0.4</v>
+      </c>
+      <c r="K15" s="68">
+        <v>51.3</v>
+      </c>
+      <c r="L15" s="51"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="57" t="s">
         <v>111</v>
       </c>
@@ -1923,24 +1987,27 @@
       <c r="E16" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="F16" s="61">
-        <v>52.5</v>
-      </c>
-      <c r="G16" s="70">
-        <v>24.1</v>
-      </c>
-      <c r="H16" s="70">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="I16" s="70">
-        <v>1.6</v>
+      <c r="F16" s="53">
+        <v>106</v>
+      </c>
+      <c r="G16" s="61">
+        <v>52.2</v>
+      </c>
+      <c r="H16" s="69">
+        <v>24.3</v>
+      </c>
+      <c r="I16" s="69">
+        <v>16.8</v>
       </c>
       <c r="J16" s="69">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="K16" s="51"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.9</v>
+      </c>
+      <c r="K16" s="68">
+        <v>16.5</v>
+      </c>
+      <c r="L16" s="51"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>126</v>
       </c>
@@ -1956,48 +2023,39 @@
       <c r="E17" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="66">
-        <v>48</v>
-      </c>
-      <c r="G17" s="71">
-        <v>23.9</v>
-      </c>
-      <c r="H17" s="71">
-        <v>13.6</v>
-      </c>
-      <c r="I17" s="71">
-        <v>0.5</v>
-      </c>
-      <c r="J17" s="71">
-        <v>18.3</v>
-      </c>
-      <c r="K17" s="51"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
+      <c r="F17" s="65">
+        <v>57.5</v>
+      </c>
+      <c r="G17" s="66">
+        <v>47</v>
+      </c>
+      <c r="H17" s="70">
+        <v>24.3</v>
+      </c>
+      <c r="I17" s="70">
+        <v>14</v>
+      </c>
+      <c r="J17" s="70">
+        <v>12.8</v>
+      </c>
+      <c r="K17" s="70">
+        <v>17.5</v>
+      </c>
+      <c r="L17" s="51"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2007,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,26 +2090,26 @@
     <col min="15" max="15" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:22" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2068,7 +2126,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2085,7 +2143,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2094,19 +2152,19 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="76" t="s">
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="76"/>
-    </row>
-    <row r="5" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="75"/>
+    </row>
+    <row r="5" spans="1:22" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -2152,8 +2210,20 @@
       <c r="P5" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V5">
+        <v>10179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -2199,8 +2269,20 @@
       <c r="P6" s="14">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
@@ -2246,8 +2328,20 @@
       <c r="P7" s="20">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
@@ -2293,8 +2387,20 @@
       <c r="P8" s="20">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V8">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
@@ -2340,8 +2446,20 @@
       <c r="P9" s="14">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>35</v>
+      </c>
+      <c r="T9" t="s">
+        <v>13</v>
+      </c>
+      <c r="U9" t="s">
+        <v>15</v>
+      </c>
+      <c r="V9">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>36</v>
       </c>
@@ -2387,8 +2505,20 @@
       <c r="P10" s="20">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" t="s">
+        <v>14</v>
+      </c>
+      <c r="U10" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -2434,8 +2564,20 @@
       <c r="P11" s="14">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" t="s">
+        <v>17</v>
+      </c>
+      <c r="U11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11">
+        <v>16395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>11</v>
       </c>
@@ -2481,8 +2623,20 @@
       <c r="P12" s="20">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>18</v>
+      </c>
+      <c r="T12" t="s">
+        <v>19</v>
+      </c>
+      <c r="U12" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
@@ -2529,7 +2683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="21"/>
       <c r="C14" s="23"/>
@@ -2546,7 +2700,7 @@
       <c r="N14" s="7"/>
       <c r="O14" s="14"/>
     </row>
-    <row r="15" spans="1:17" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>67</v>
       </c>
@@ -2585,7 +2739,7 @@
       </c>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>37</v>
       </c>
@@ -2884,6 +3038,11 @@
         <v>49</v>
       </c>
     </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>141</v>
+      </c>
+    </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>43</v>
@@ -2895,7 +3054,11 @@
         <v>6</v>
       </c>
       <c r="D29" s="29">
-        <v>46.878782800000003</v>
+        <v>18.100000000000001</v>
+      </c>
+      <c r="F29">
+        <f>D29*1.60934^2</f>
+        <v>46.878551764360004</v>
       </c>
       <c r="G29" s="30">
         <v>0.43041607439999996</v>
@@ -2918,7 +3081,11 @@
         <v>6</v>
       </c>
       <c r="D30" s="31">
-        <v>318.56852399999997</v>
+        <v>123</v>
+      </c>
+      <c r="F30">
+        <f>D30*1.60934^2</f>
+        <v>318.56695397879997</v>
       </c>
       <c r="G30" s="30">
         <v>3.0015857819999998</v>
@@ -2941,7 +3108,11 @@
         <v>6</v>
       </c>
       <c r="D31" s="31">
-        <v>378.13824799999998</v>
+        <v>146</v>
+      </c>
+      <c r="F31">
+        <f>D31*1.60934^2</f>
+        <v>378.13638439759995</v>
       </c>
       <c r="G31" s="30">
         <v>5.2244582714999996</v>
@@ -2975,6 +3146,10 @@
       <c r="E33" t="s">
         <v>62</v>
       </c>
+      <c r="F33">
+        <f>D33*1.60934^2</f>
+        <v>1572.1149680091999</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
@@ -2992,6 +3167,10 @@
       <c r="E34" t="s">
         <v>62</v>
       </c>
+      <c r="F34">
+        <f>D34*1.60934^2</f>
+        <v>78.21725211511999</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -3006,6 +3185,10 @@
       <c r="E37" t="s">
         <v>62</v>
       </c>
+      <c r="F37">
+        <f t="shared" ref="F37:F39" si="0">D37*1.60934^2</f>
+        <v>47.914541858599996</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -3023,6 +3206,10 @@
       <c r="E38" t="s">
         <v>62</v>
       </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>106.1889846596</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -3036,6 +3223,10 @@
       </c>
       <c r="E39" t="s">
         <v>62</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>57.497450230319998</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>